<commit_message>
remove multiple samples honeybee
</commit_message>
<xml_diff>
--- a/tblshoot/ThreeMethods/compare3.xlsx
+++ b/tblshoot/ThreeMethods/compare3.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindz/BeeVirusDiet/tblshoot/ThreeMethods/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="0" windowWidth="12640" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="2420" yWindow="460" windowWidth="12640" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -218,6 +226,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -546,10 +559,10 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
@@ -560,7 +573,7 @@
     <col min="9" max="10" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +605,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -624,11 +637,11 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <f>AVERAGE(B2,E2,H2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <f t="shared" ref="K2:K29" si="0">AVERAGE(B2,E2,H2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -660,11 +673,11 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <f>AVERAGE(B3,E3,H3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -696,11 +709,11 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <f>AVERAGE(B4,E4,H4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -732,11 +745,11 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <f>AVERAGE(B5,E5,H5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -768,11 +781,11 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <f>AVERAGE(B6,E6,H6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -804,11 +817,11 @@
         <v>2</v>
       </c>
       <c r="K7">
-        <f>AVERAGE(B7,E7,H7)</f>
+        <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -840,11 +853,11 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <f>AVERAGE(B8,E8,H8)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -876,11 +889,11 @@
         <v>1</v>
       </c>
       <c r="K9">
-        <f>AVERAGE(B9,E9,H9)</f>
+        <f t="shared" si="0"/>
         <v>19.666666666666668</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -912,11 +925,11 @@
         <v>12</v>
       </c>
       <c r="K10">
-        <f>AVERAGE(B10,E10,H10)</f>
+        <f t="shared" si="0"/>
         <v>23.666666666666668</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -948,11 +961,11 @@
         <v>8</v>
       </c>
       <c r="K11">
-        <f>AVERAGE(B11,E11,H11)</f>
+        <f t="shared" si="0"/>
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -984,11 +997,11 @@
         <v>22</v>
       </c>
       <c r="K12">
-        <f>AVERAGE(B12,E12,H12)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1020,11 +1033,11 @@
         <v>5</v>
       </c>
       <c r="K13">
-        <f>AVERAGE(B13,E13,H13)</f>
+        <f t="shared" si="0"/>
         <v>71.333333333333329</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1056,11 +1069,11 @@
         <v>62</v>
       </c>
       <c r="K14">
-        <f>AVERAGE(B14,E14,H14)</f>
+        <f t="shared" si="0"/>
         <v>73.666666666666671</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1092,11 +1105,11 @@
         <v>8</v>
       </c>
       <c r="K15">
-        <f>AVERAGE(B15,E15,H15)</f>
+        <f t="shared" si="0"/>
         <v>76.666666666666671</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="4" customFormat="1">
+    <row r="16" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1128,11 +1141,11 @@
         <v>85</v>
       </c>
       <c r="K16" s="4">
-        <f>AVERAGE(B16,E16,H16)</f>
+        <f t="shared" si="0"/>
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1164,11 +1177,11 @@
         <v>60</v>
       </c>
       <c r="K17">
-        <f>AVERAGE(B17,E17,H17)</f>
+        <f t="shared" si="0"/>
         <v>142.66666666666666</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
@@ -1200,11 +1213,11 @@
         <v>94</v>
       </c>
       <c r="K18">
-        <f>AVERAGE(B18,E18,H18)</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -1236,11 +1249,11 @@
         <v>137</v>
       </c>
       <c r="K19">
-        <f>AVERAGE(B19,E19,H19)</f>
+        <f t="shared" si="0"/>
         <v>322.66666666666669</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1272,11 +1285,11 @@
         <v>192</v>
       </c>
       <c r="K20">
-        <f>AVERAGE(B20,E20,H20)</f>
+        <f t="shared" si="0"/>
         <v>402.33333333333331</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1308,11 +1321,11 @@
         <v>215</v>
       </c>
       <c r="K21">
-        <f>AVERAGE(B21,E21,H21)</f>
+        <f t="shared" si="0"/>
         <v>431.66666666666669</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="4" customFormat="1">
+    <row r="22" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>15</v>
       </c>
@@ -1344,11 +1357,11 @@
         <v>354</v>
       </c>
       <c r="K22" s="4">
-        <f>AVERAGE(B22,E22,H22)</f>
+        <f t="shared" si="0"/>
         <v>618</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1380,11 +1393,11 @@
         <v>295</v>
       </c>
       <c r="K23">
-        <f>AVERAGE(B23,E23,H23)</f>
+        <f t="shared" si="0"/>
         <v>696.33333333333337</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1416,11 +1429,11 @@
         <v>58</v>
       </c>
       <c r="K24">
-        <f>AVERAGE(B24,E24,H24)</f>
+        <f t="shared" si="0"/>
         <v>760.33333333333337</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1452,11 +1465,11 @@
         <v>371</v>
       </c>
       <c r="K25">
-        <f>AVERAGE(B25,E25,H25)</f>
+        <f t="shared" si="0"/>
         <v>1350</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>18</v>
       </c>
@@ -1488,11 +1501,11 @@
         <v>888</v>
       </c>
       <c r="K26">
-        <f>AVERAGE(B26,E26,H26)</f>
+        <f t="shared" si="0"/>
         <v>1930.3333333333333</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -1524,11 +1537,11 @@
         <v>1219</v>
       </c>
       <c r="K27">
-        <f>AVERAGE(B27,E27,H27)</f>
+        <f t="shared" si="0"/>
         <v>1987.6666666666667</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
@@ -1560,11 +1573,11 @@
         <v>2058</v>
       </c>
       <c r="K28">
-        <f>AVERAGE(B28,E28,H28)</f>
+        <f t="shared" si="0"/>
         <v>2339.3333333333335</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1596,7 +1609,7 @@
         <v>1372</v>
       </c>
       <c r="K29">
-        <f>AVERAGE(B29,E29,H29)</f>
+        <f t="shared" si="0"/>
         <v>2585.3333333333335</v>
       </c>
     </row>
@@ -1606,10 +1619,5 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Form data for four treatment subsets
</commit_message>
<xml_diff>
--- a/tblshoot/ThreeMethods/compare3.xlsx
+++ b/tblshoot/ThreeMethods/compare3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="460" windowWidth="12640" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="5360" yWindow="460" windowWidth="18940" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>limma</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>btwnLane-edgeR</t>
   </si>
 </sst>
 </file>
@@ -172,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,18 +185,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF008000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF3366FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,11 +203,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -556,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,9 +560,10 @@
     <col min="6" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -602,11 +592,14 @@
         <v>36</v>
       </c>
       <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1">
@@ -637,12 +630,15 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K29" si="0">AVERAGE(B2,E2,H2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(B2:K2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
@@ -673,12 +669,15 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f>AVERAGE(B3:K3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="1">
@@ -709,12 +708,15 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>AVERAGE(B4:K4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="1">
@@ -745,12 +747,15 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f>AVERAGE(B5:K5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="1">
@@ -781,12 +786,15 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f>AVERAGE(B6:K6)</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1">
@@ -817,11 +825,14 @@
         <v>2</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f>AVERAGE(B7:K7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -853,12 +864,15 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f>AVERAGE(B8:K8)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="1">
@@ -889,480 +903,522 @@
         <v>1</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
-        <v>19.666666666666668</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f>AVERAGE(B9:K9)</f>
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="F10">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G10">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="H10" s="1">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J10">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
-        <v>23.666666666666668</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <f>AVERAGE(B10:K10)</f>
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F11">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G11">
+        <v>65</v>
+      </c>
+      <c r="H11" s="1">
+        <v>24</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>22</v>
+      </c>
+      <c r="K11">
+        <v>72</v>
+      </c>
+      <c r="L11">
+        <f>AVERAGE(B11:K11)</f>
+        <v>28.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>132</v>
+      </c>
+      <c r="F12">
+        <v>117</v>
+      </c>
+      <c r="G12">
+        <v>15</v>
+      </c>
+      <c r="H12" s="1">
+        <v>82</v>
+      </c>
+      <c r="I12">
+        <v>77</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <v>233</v>
+      </c>
+      <c r="L12">
+        <f>AVERAGE(B12:K12)</f>
+        <v>66.099999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>155</v>
+      </c>
+      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="G13">
+        <v>147</v>
+      </c>
+      <c r="H13" s="1">
         <v>66</v>
       </c>
-      <c r="H11" s="1">
-        <v>13</v>
-      </c>
-      <c r="I11">
-        <v>5</v>
-      </c>
-      <c r="J11">
-        <v>8</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>33.333333333333336</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12" s="1">
-        <v>78</v>
-      </c>
-      <c r="F12">
-        <v>13</v>
-      </c>
-      <c r="G12">
-        <v>65</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>62</v>
+      </c>
+      <c r="K13">
+        <v>265</v>
+      </c>
+      <c r="L13">
+        <f>AVERAGE(B13:K13)</f>
+        <v>70.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
-      <c r="J12">
-        <v>22</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>132</v>
-      </c>
-      <c r="F13">
-        <v>117</v>
-      </c>
-      <c r="G13">
-        <v>15</v>
-      </c>
-      <c r="H13" s="1">
-        <v>82</v>
-      </c>
-      <c r="I13">
-        <v>77</v>
-      </c>
-      <c r="J13">
-        <v>5</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>71.333333333333329</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
       <c r="B14" s="1">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E14" s="1">
-        <v>155</v>
+        <v>225</v>
       </c>
       <c r="F14">
-        <v>8</v>
+        <v>137</v>
       </c>
       <c r="G14">
-        <v>147</v>
+        <v>88</v>
       </c>
       <c r="H14" s="1">
-        <v>66</v>
+        <v>151</v>
       </c>
       <c r="I14">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="J14">
-        <v>62</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
-        <v>73.666666666666671</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>27</v>
+        <v>60</v>
+      </c>
+      <c r="K14" s="2">
+        <v>178</v>
+      </c>
+      <c r="L14">
+        <f>AVERAGE(B14:K14)</f>
+        <v>103.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E15" s="1">
-        <v>207</v>
+        <v>284</v>
       </c>
       <c r="F15">
-        <v>182</v>
+        <v>142</v>
       </c>
       <c r="G15">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="H15" s="1">
-        <v>23</v>
+        <v>206</v>
       </c>
       <c r="I15">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="J15">
-        <v>8</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>76.666666666666671</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f>AVERAGE(B15:K15)</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>9</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="2">
         <v>1</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="2">
         <v>8</v>
       </c>
       <c r="E16" s="1">
         <v>217</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="2">
         <v>41</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="2">
         <v>176</v>
       </c>
       <c r="H16" s="1">
         <v>113</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="2">
         <v>27</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="2">
         <v>85</v>
       </c>
-      <c r="K16" s="4">
-        <f t="shared" si="0"/>
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>24</v>
+      <c r="K16" s="2">
+        <v>552</v>
+      </c>
+      <c r="L16">
+        <f>AVERAGE(B16:K16)</f>
+        <v>122.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B17" s="1">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E17" s="1">
-        <v>225</v>
+        <v>51</v>
       </c>
       <c r="F17">
+        <v>18</v>
+      </c>
+      <c r="G17">
+        <v>33</v>
+      </c>
+      <c r="H17" s="1">
+        <v>19</v>
+      </c>
+      <c r="I17">
+        <v>7</v>
+      </c>
+      <c r="J17">
+        <v>12</v>
+      </c>
+      <c r="K17">
+        <v>1623</v>
+      </c>
+      <c r="L17">
+        <f>AVERAGE(B17:K17)</f>
+        <v>176.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1">
+        <v>26</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1">
+        <v>747</v>
+      </c>
+      <c r="F18">
+        <v>451</v>
+      </c>
+      <c r="G18">
+        <v>296</v>
+      </c>
+      <c r="H18" s="1">
+        <v>434</v>
+      </c>
+      <c r="I18">
+        <v>242</v>
+      </c>
+      <c r="J18">
+        <v>192</v>
+      </c>
+      <c r="K18">
+        <v>18</v>
+      </c>
+      <c r="L18">
+        <f>AVERAGE(B18:K18)</f>
+        <v>243.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>207</v>
+      </c>
+      <c r="F19">
+        <v>182</v>
+      </c>
+      <c r="G19">
+        <v>25</v>
+      </c>
+      <c r="H19" s="1">
+        <v>23</v>
+      </c>
+      <c r="I19">
+        <v>15</v>
+      </c>
+      <c r="J19">
+        <v>8</v>
+      </c>
+      <c r="K19">
+        <v>2321</v>
+      </c>
+      <c r="L19">
+        <f>AVERAGE(B19:K19)</f>
+        <v>278.10000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1">
+        <v>189</v>
+      </c>
+      <c r="C20">
+        <v>103</v>
+      </c>
+      <c r="D20">
+        <v>86</v>
+      </c>
+      <c r="E20" s="1">
+        <v>628</v>
+      </c>
+      <c r="F20">
+        <v>353</v>
+      </c>
+      <c r="G20">
+        <v>275</v>
+      </c>
+      <c r="H20" s="1">
+        <v>478</v>
+      </c>
+      <c r="I20">
+        <v>263</v>
+      </c>
+      <c r="J20">
+        <v>215</v>
+      </c>
+      <c r="K20">
+        <v>219</v>
+      </c>
+      <c r="L20">
+        <f>AVERAGE(B20:K20)</f>
+        <v>280.89999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>572</v>
+      </c>
+      <c r="F21">
+        <v>440</v>
+      </c>
+      <c r="G21">
+        <v>132</v>
+      </c>
+      <c r="H21" s="1">
+        <v>396</v>
+      </c>
+      <c r="I21">
+        <v>259</v>
+      </c>
+      <c r="J21">
         <v>137</v>
       </c>
-      <c r="G17">
-        <v>88</v>
-      </c>
-      <c r="H17" s="1">
-        <v>151</v>
-      </c>
-      <c r="I17">
-        <v>91</v>
-      </c>
-      <c r="J17">
-        <v>60</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>142.66666666666666</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="1">
-        <v>50</v>
-      </c>
-      <c r="C18">
-        <v>25</v>
-      </c>
-      <c r="D18">
-        <v>25</v>
-      </c>
-      <c r="E18" s="1">
-        <v>284</v>
-      </c>
-      <c r="F18">
-        <v>142</v>
-      </c>
-      <c r="G18">
-        <v>142</v>
-      </c>
-      <c r="H18" s="1">
-        <v>206</v>
-      </c>
-      <c r="I18">
-        <v>112</v>
-      </c>
-      <c r="J18">
-        <v>94</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>572</v>
-      </c>
-      <c r="F19">
-        <v>440</v>
-      </c>
-      <c r="G19">
-        <v>132</v>
-      </c>
-      <c r="H19" s="1">
-        <v>396</v>
-      </c>
-      <c r="I19">
-        <v>259</v>
-      </c>
-      <c r="J19">
-        <v>137</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>322.66666666666669</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="1">
-        <v>26</v>
-      </c>
-      <c r="C20">
-        <v>17</v>
-      </c>
-      <c r="D20">
-        <v>9</v>
-      </c>
-      <c r="E20" s="1">
-        <v>747</v>
-      </c>
-      <c r="F20">
-        <v>451</v>
-      </c>
-      <c r="G20">
-        <v>296</v>
-      </c>
-      <c r="H20" s="1">
-        <v>434</v>
-      </c>
-      <c r="I20">
-        <v>242</v>
-      </c>
-      <c r="J20">
-        <v>192</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="0"/>
-        <v>402.33333333333331</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="1">
-        <v>189</v>
-      </c>
-      <c r="C21">
-        <v>103</v>
-      </c>
-      <c r="D21">
-        <v>86</v>
-      </c>
-      <c r="E21" s="1">
-        <v>628</v>
-      </c>
-      <c r="F21">
-        <v>353</v>
-      </c>
-      <c r="G21">
-        <v>275</v>
-      </c>
-      <c r="H21" s="1">
-        <v>478</v>
-      </c>
-      <c r="I21">
-        <v>263</v>
-      </c>
-      <c r="J21">
-        <v>215</v>
-      </c>
       <c r="K21">
-        <f t="shared" si="0"/>
-        <v>431.66666666666669</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+        <v>1080</v>
+      </c>
+      <c r="L21">
+        <f>AVERAGE(B21:K21)</f>
+        <v>301.60000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="1">
         <v>562</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="2">
         <v>259</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="2">
         <v>303</v>
       </c>
       <c r="E22" s="1">
         <v>717</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="2">
         <v>286</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="2">
         <v>431</v>
       </c>
       <c r="H22" s="1">
         <v>575</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="2">
         <v>221</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="2">
         <v>354</v>
       </c>
-      <c r="K22" s="4">
-        <f t="shared" si="0"/>
-        <v>618</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="K22" s="2">
+        <v>3</v>
+      </c>
+      <c r="L22">
+        <f>AVERAGE(B22:K22)</f>
+        <v>371.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="1">
@@ -1393,12 +1449,15 @@
         <v>295</v>
       </c>
       <c r="K23">
-        <f t="shared" si="0"/>
-        <v>696.33333333333337</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <f>AVERAGE(B23:K23)</f>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="1">
@@ -1429,83 +1488,92 @@
         <v>58</v>
       </c>
       <c r="K24">
-        <f t="shared" si="0"/>
-        <v>760.33333333333337</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+        <v>6319</v>
+      </c>
+      <c r="L24">
+        <f>AVERAGE(B24:K24)</f>
+        <v>1087.9000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1824</v>
+      </c>
+      <c r="C25">
+        <v>952</v>
+      </c>
+      <c r="D25">
+        <v>872</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2166</v>
+      </c>
+      <c r="F25">
+        <v>1019</v>
+      </c>
+      <c r="G25">
+        <v>1147</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1801</v>
+      </c>
+      <c r="I25">
+        <v>913</v>
+      </c>
+      <c r="J25">
+        <v>888</v>
+      </c>
+      <c r="K25">
+        <v>74</v>
+      </c>
+      <c r="L25">
+        <f>AVERAGE(B25:K25)</f>
+        <v>1165.5999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B26" s="1">
         <v>1204</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>534</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <v>670</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E26" s="1">
         <v>1505</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <v>715</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <v>790</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H26" s="1">
         <v>1341</v>
       </c>
-      <c r="I25">
+      <c r="I26">
         <v>966</v>
       </c>
-      <c r="J25">
+      <c r="J26">
         <v>371</v>
       </c>
-      <c r="K25">
-        <f t="shared" si="0"/>
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1824</v>
-      </c>
-      <c r="C26">
-        <v>952</v>
-      </c>
-      <c r="D26">
-        <v>872</v>
-      </c>
-      <c r="E26" s="1">
-        <v>2166</v>
-      </c>
-      <c r="F26">
-        <v>1019</v>
-      </c>
-      <c r="G26">
-        <v>1147</v>
-      </c>
-      <c r="H26" s="1">
-        <v>1801</v>
-      </c>
-      <c r="I26">
-        <v>913</v>
-      </c>
-      <c r="J26">
-        <v>888</v>
-      </c>
       <c r="K26">
-        <f t="shared" si="0"/>
-        <v>1930.3333333333333</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+        <v>5753</v>
+      </c>
+      <c r="L26">
+        <f>AVERAGE(B26:K26)</f>
+        <v>1384.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -1537,85 +1605,94 @@
         <v>1219</v>
       </c>
       <c r="K27">
-        <f t="shared" si="0"/>
-        <v>1987.6666666666667</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2467</v>
+      </c>
+      <c r="L27">
+        <f>AVERAGE(B27:K27)</f>
+        <v>1439.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2551</v>
+      </c>
+      <c r="C28">
+        <v>1314</v>
+      </c>
+      <c r="D28">
+        <v>1237</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2761</v>
+      </c>
+      <c r="F28">
+        <v>1300</v>
+      </c>
+      <c r="G28">
+        <v>1461</v>
+      </c>
+      <c r="H28" s="1">
+        <v>2444</v>
+      </c>
+      <c r="I28">
+        <v>1068</v>
+      </c>
+      <c r="J28">
+        <v>1372</v>
+      </c>
+      <c r="K28">
+        <v>2523</v>
+      </c>
+      <c r="L28">
+        <f>AVERAGE(B28:K28)</f>
+        <v>1803.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B29" s="1">
         <v>1743</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>1088</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>655</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E29" s="1">
         <v>2811</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <v>1620</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>1191</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H29" s="1">
         <v>2464</v>
       </c>
-      <c r="I28">
+      <c r="I29">
         <v>405</v>
       </c>
-      <c r="J28">
+      <c r="J29">
         <v>2058</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="0"/>
-        <v>2339.3333333333335</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="1">
-        <v>2551</v>
-      </c>
-      <c r="C29">
-        <v>1314</v>
-      </c>
-      <c r="D29">
-        <v>1237</v>
-      </c>
-      <c r="E29" s="1">
-        <v>2761</v>
-      </c>
-      <c r="F29">
-        <v>1300</v>
-      </c>
-      <c r="G29">
-        <v>1461</v>
-      </c>
-      <c r="H29" s="1">
-        <v>2444</v>
-      </c>
-      <c r="I29">
-        <v>1068</v>
-      </c>
-      <c r="J29">
-        <v>1372</v>
-      </c>
       <c r="K29">
-        <f t="shared" si="0"/>
-        <v>2585.3333333333335</v>
+        <v>5383</v>
+      </c>
+      <c r="L29">
+        <f>AVERAGE(B29:K29)</f>
+        <v>1941.8</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:K29">
-    <sortCondition ref="K2:K29"/>
+  <sortState ref="A2:L29">
+    <sortCondition ref="L2:L29"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>